<commit_message>
optimizers and citations added
</commit_message>
<xml_diff>
--- a/Chapters/Figures/conv-example.xlsx
+++ b/Chapters/Figures/conv-example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Documents\Grad_School\BNL_Thesis\Chapters\Figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FF6CD3-61F6-4B7F-BE7B-635247C50AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B696BF7E-5437-486C-86A8-55511BA47096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6312" yWindow="1344" windowWidth="15204" windowHeight="10368" xr2:uid="{BC617ED9-BD49-44FE-8959-C0D256CDD9D5}"/>
   </bookViews>
@@ -932,7 +932,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -2662,6 +2662,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
figures and a little writing. backing up
</commit_message>
<xml_diff>
--- a/Chapters/Figures/conv-example.xlsx
+++ b/Chapters/Figures/conv-example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Documents\Grad_School\BNL_Thesis\Chapters\Figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B696BF7E-5437-486C-86A8-55511BA47096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC83DB0-A890-479D-9137-99B094F72B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6312" yWindow="1344" windowWidth="15204" windowHeight="10368" xr2:uid="{BC617ED9-BD49-44FE-8959-C0D256CDD9D5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{BC617ED9-BD49-44FE-8959-C0D256CDD9D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -293,6 +293,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Energy, E</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -355,6 +410,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Absorption</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2053,16 +2163,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>499110</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>445770</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>194310</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>140970</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2425,8 +2535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1EA0053-12BD-416B-90C7-7240D9DAB9A1}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>